<commit_message>
using UNCTAD source for FDI
</commit_message>
<xml_diff>
--- a/series_list.xlsx
+++ b/series_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\EADS Requests\2020_03_31 Michael Nicholson - Africa Poverty Research\Edited data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B72342C-8976-4DD5-8818-BECD584D9ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDE86D-512D-42F2-B9A4-9E3A31ED7571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3250E18-4E32-4277-BA3D-2DC744EC6245}"/>
+    <workbookView xWindow="1170" yWindow="960" windowWidth="23700" windowHeight="15240" xr2:uid="{F3250E18-4E32-4277-BA3D-2DC744EC6245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>fdi</t>
   </si>
   <si>
-    <t>U.S. Direct Investment Abroad: Direct investment position ($US millions, historical-cost basis)</t>
-  </si>
-  <si>
     <t>Legatum Prosperity Index: Education Score (0-100, higher is better)</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>infrastructure</t>
+  </si>
+  <si>
+    <t>Foreign direct investment (FDI)  inflows ($US millions)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +706,7 @@
         <v>65821</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -717,16 +717,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>704</v>
+        <v>1665</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,10 +734,10 @@
         <v>70538</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
       </c>
       <c r="D13">
         <v>165</v>

</xml_diff>